<commit_message>
move overview plots to page eda
</commit_message>
<xml_diff>
--- a/data/flight_dataset_description.xlsx
+++ b/data/flight_dataset_description.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>Column Name</t>
   </si>
@@ -872,6 +872,9 @@
   </si>
   <si>
     <t>No filter</t>
+  </si>
+  <si>
+    <t>(Select one)</t>
   </si>
 </sst>
 </file>
@@ -2140,39 +2143,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A13:C22"/>
+  <dimension ref="A13:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="13"/>
+    <col min="2" max="2" width="14" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D13" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>144</v>
       </c>

</xml_diff>